<commit_message>
batch 1 rep 7 to 10
</commit_message>
<xml_diff>
--- a/data/Grain_Counting/gc_57_1.xlsx
+++ b/data/Grain_Counting/gc_57_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/han-wenhsu/Library/Mobile Documents/com~apple~CloudDocs/HU Dokumente/6. Semester/Studienprojekt/Ear_development_BSC_project_hwh/data/Grain_Counting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40513F97-3C57-1B43-B9B7-A0F528D8DBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B067448-EFAC-C144-9D98-6386B2B66F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rep1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,10 @@
     <sheet name="rep4" sheetId="13" r:id="rId4"/>
     <sheet name="rep5" sheetId="14" r:id="rId5"/>
     <sheet name="rep6" sheetId="15" r:id="rId6"/>
+    <sheet name="rep7" sheetId="16" r:id="rId7"/>
+    <sheet name="rep8" sheetId="17" r:id="rId8"/>
+    <sheet name="rep9" sheetId="18" r:id="rId9"/>
+    <sheet name="rep10" sheetId="19" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="12">
   <si>
     <t>var</t>
   </si>
@@ -250,13 +254,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -292,6 +293,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -307,10 +311,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -961,6 +961,445 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA2D27D-DC75-8B45-95F4-CCE9A1F7B091}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14">
+        <v>57</v>
+      </c>
+      <c r="C2" s="14">
+        <v>10</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="14">
+        <v>57</v>
+      </c>
+      <c r="C3" s="14">
+        <v>10</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2</v>
+      </c>
+      <c r="E3" s="16">
+        <v>5</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="14">
+        <v>57</v>
+      </c>
+      <c r="C4" s="14">
+        <v>10</v>
+      </c>
+      <c r="D4" s="15">
+        <v>3</v>
+      </c>
+      <c r="E4" s="16">
+        <v>5</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="14">
+        <v>57</v>
+      </c>
+      <c r="C5" s="14">
+        <v>10</v>
+      </c>
+      <c r="D5" s="15">
+        <v>4</v>
+      </c>
+      <c r="E5" s="16">
+        <v>5</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14">
+        <v>57</v>
+      </c>
+      <c r="C6" s="14">
+        <v>10</v>
+      </c>
+      <c r="D6" s="15">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <v>6</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="14">
+        <v>57</v>
+      </c>
+      <c r="C7" s="14">
+        <v>10</v>
+      </c>
+      <c r="D7" s="15">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16">
+        <v>6</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14">
+        <v>57</v>
+      </c>
+      <c r="C8" s="14">
+        <v>10</v>
+      </c>
+      <c r="D8" s="15">
+        <v>7</v>
+      </c>
+      <c r="E8" s="16">
+        <v>6</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14">
+        <v>57</v>
+      </c>
+      <c r="C9" s="14">
+        <v>10</v>
+      </c>
+      <c r="D9" s="15">
+        <v>8</v>
+      </c>
+      <c r="E9" s="16">
+        <v>6</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>57</v>
+      </c>
+      <c r="C10" s="14">
+        <v>10</v>
+      </c>
+      <c r="D10" s="15">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16">
+        <v>6</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14">
+        <v>10</v>
+      </c>
+      <c r="D11" s="15">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16">
+        <v>6</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14">
+        <v>57</v>
+      </c>
+      <c r="C12" s="14">
+        <v>10</v>
+      </c>
+      <c r="D12" s="15">
+        <v>11</v>
+      </c>
+      <c r="E12" s="16">
+        <v>6</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14">
+        <v>57</v>
+      </c>
+      <c r="C13" s="14">
+        <v>10</v>
+      </c>
+      <c r="D13" s="15">
+        <v>12</v>
+      </c>
+      <c r="E13" s="16">
+        <v>6</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="14">
+        <v>57</v>
+      </c>
+      <c r="C14" s="14">
+        <v>10</v>
+      </c>
+      <c r="D14" s="15">
+        <v>13</v>
+      </c>
+      <c r="E14" s="16">
+        <v>6</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="14">
+        <v>57</v>
+      </c>
+      <c r="C15" s="14">
+        <v>10</v>
+      </c>
+      <c r="D15" s="15">
+        <v>14</v>
+      </c>
+      <c r="E15" s="16">
+        <v>5</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="14">
+        <v>57</v>
+      </c>
+      <c r="C16" s="14">
+        <v>10</v>
+      </c>
+      <c r="D16" s="15">
+        <v>15</v>
+      </c>
+      <c r="E16" s="16">
+        <v>5</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="14">
+        <v>57</v>
+      </c>
+      <c r="C17" s="14">
+        <v>10</v>
+      </c>
+      <c r="D17" s="15">
+        <v>16</v>
+      </c>
+      <c r="E17" s="16">
+        <v>5</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="14">
+        <v>57</v>
+      </c>
+      <c r="C18" s="14">
+        <v>10</v>
+      </c>
+      <c r="D18" s="15">
+        <v>17</v>
+      </c>
+      <c r="E18" s="16">
+        <v>5</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="14">
+        <v>57</v>
+      </c>
+      <c r="C19" s="14">
+        <v>10</v>
+      </c>
+      <c r="D19" s="15">
+        <v>18</v>
+      </c>
+      <c r="E19" s="16">
+        <v>5</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="14">
+        <v>57</v>
+      </c>
+      <c r="C20" s="14">
+        <v>10</v>
+      </c>
+      <c r="D20" s="15">
+        <v>19</v>
+      </c>
+      <c r="E20" s="16">
+        <v>4</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="14">
+        <v>57</v>
+      </c>
+      <c r="C21" s="14">
+        <v>10</v>
+      </c>
+      <c r="D21" s="15">
+        <v>20</v>
+      </c>
+      <c r="E21" s="19">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD609FEA-AE2C-1F4E-8053-DF41718EC9A1}">
   <dimension ref="A1:H20"/>
@@ -972,7 +1411,6 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="10.83203125" style="8"/>
     <col min="6" max="8" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -1342,7 +1780,6 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="10.83203125" style="8"/>
     <col min="6" max="8" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -1698,7 +2135,6 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="10.83203125" style="8"/>
     <col min="6" max="8" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -2057,407 +2493,407 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="13" t="s">
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="15">
-        <v>57</v>
-      </c>
-      <c r="C2" s="15">
-        <v>5</v>
-      </c>
-      <c r="D2" s="16">
+      <c r="A2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14">
+        <v>57</v>
+      </c>
+      <c r="C2" s="14">
+        <v>5</v>
+      </c>
+      <c r="D2" s="15">
         <v>1</v>
       </c>
-      <c r="E2" s="17">
-        <v>4</v>
-      </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="E2" s="16">
+        <v>4</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="15">
-        <v>57</v>
-      </c>
-      <c r="C3" s="15">
-        <v>5</v>
-      </c>
-      <c r="D3" s="16">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="14">
+        <v>57</v>
+      </c>
+      <c r="C3" s="14">
+        <v>5</v>
+      </c>
+      <c r="D3" s="15">
         <v>2</v>
       </c>
-      <c r="E3" s="17">
-        <v>5</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="E3" s="16">
+        <v>5</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="15">
-        <v>57</v>
-      </c>
-      <c r="C4" s="15">
-        <v>5</v>
-      </c>
-      <c r="D4" s="16">
+      <c r="A4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="14">
+        <v>57</v>
+      </c>
+      <c r="C4" s="14">
+        <v>5</v>
+      </c>
+      <c r="D4" s="15">
         <v>3</v>
       </c>
-      <c r="E4" s="17">
-        <v>5</v>
-      </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="16">
+        <v>5</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="15">
-        <v>57</v>
-      </c>
-      <c r="C5" s="15">
-        <v>5</v>
-      </c>
-      <c r="D5" s="16">
-        <v>4</v>
-      </c>
-      <c r="E5" s="17">
-        <v>5</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="A5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="14">
+        <v>57</v>
+      </c>
+      <c r="C5" s="14">
+        <v>5</v>
+      </c>
+      <c r="D5" s="15">
+        <v>4</v>
+      </c>
+      <c r="E5" s="16">
+        <v>5</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="15">
-        <v>57</v>
-      </c>
-      <c r="C6" s="15">
-        <v>5</v>
-      </c>
-      <c r="D6" s="16">
-        <v>5</v>
-      </c>
-      <c r="E6" s="17">
-        <v>6</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14">
+        <v>57</v>
+      </c>
+      <c r="C6" s="14">
+        <v>5</v>
+      </c>
+      <c r="D6" s="15">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <v>6</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="15">
-        <v>57</v>
-      </c>
-      <c r="C7" s="15">
-        <v>5</v>
-      </c>
-      <c r="D7" s="16">
-        <v>6</v>
-      </c>
-      <c r="E7" s="17">
-        <v>6</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="A7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="14">
+        <v>57</v>
+      </c>
+      <c r="C7" s="14">
+        <v>5</v>
+      </c>
+      <c r="D7" s="15">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16">
+        <v>6</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="15">
-        <v>57</v>
-      </c>
-      <c r="C8" s="15">
-        <v>5</v>
-      </c>
-      <c r="D8" s="16">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14">
+        <v>57</v>
+      </c>
+      <c r="C8" s="14">
+        <v>5</v>
+      </c>
+      <c r="D8" s="15">
         <v>7</v>
       </c>
-      <c r="E8" s="17">
-        <v>6</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="E8" s="16">
+        <v>6</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="15">
-        <v>57</v>
-      </c>
-      <c r="C9" s="15">
-        <v>5</v>
-      </c>
-      <c r="D9" s="16">
+      <c r="A9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14">
+        <v>57</v>
+      </c>
+      <c r="C9" s="14">
+        <v>5</v>
+      </c>
+      <c r="D9" s="15">
         <v>8</v>
       </c>
-      <c r="E9" s="17">
-        <v>6</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="E9" s="16">
+        <v>6</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="15">
-        <v>57</v>
-      </c>
-      <c r="C10" s="15">
-        <v>5</v>
-      </c>
-      <c r="D10" s="16">
-        <v>9</v>
-      </c>
-      <c r="E10" s="17">
-        <v>6</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="A10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>57</v>
+      </c>
+      <c r="C10" s="14">
+        <v>5</v>
+      </c>
+      <c r="D10" s="15">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16">
+        <v>6</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="15">
-        <v>57</v>
-      </c>
-      <c r="C11" s="15">
-        <v>5</v>
-      </c>
-      <c r="D11" s="16">
-        <v>10</v>
-      </c>
-      <c r="E11" s="17">
-        <v>6</v>
-      </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+      <c r="A11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14">
+        <v>5</v>
+      </c>
+      <c r="D11" s="15">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16">
+        <v>6</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="15">
-        <v>57</v>
-      </c>
-      <c r="C12" s="15">
-        <v>5</v>
-      </c>
-      <c r="D12" s="16">
+      <c r="A12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14">
+        <v>57</v>
+      </c>
+      <c r="C12" s="14">
+        <v>5</v>
+      </c>
+      <c r="D12" s="15">
         <v>11</v>
       </c>
-      <c r="E12" s="17">
-        <v>6</v>
-      </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="E12" s="16">
+        <v>6</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="15">
-        <v>57</v>
-      </c>
-      <c r="C13" s="15">
-        <v>5</v>
-      </c>
-      <c r="D13" s="16">
+      <c r="A13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14">
+        <v>57</v>
+      </c>
+      <c r="C13" s="14">
+        <v>5</v>
+      </c>
+      <c r="D13" s="15">
         <v>12</v>
       </c>
-      <c r="E13" s="17">
-        <v>5</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="E13" s="16">
+        <v>5</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="15">
-        <v>57</v>
-      </c>
-      <c r="C14" s="15">
-        <v>5</v>
-      </c>
-      <c r="D14" s="16">
+      <c r="A14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="14">
+        <v>57</v>
+      </c>
+      <c r="C14" s="14">
+        <v>5</v>
+      </c>
+      <c r="D14" s="15">
         <v>13</v>
       </c>
-      <c r="E14" s="17">
-        <v>5</v>
-      </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="E14" s="16">
+        <v>5</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="15">
-        <v>57</v>
-      </c>
-      <c r="C15" s="15">
-        <v>5</v>
-      </c>
-      <c r="D15" s="16">
+      <c r="A15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="14">
+        <v>57</v>
+      </c>
+      <c r="C15" s="14">
+        <v>5</v>
+      </c>
+      <c r="D15" s="15">
         <v>14</v>
       </c>
-      <c r="E15" s="17">
-        <v>5</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="E15" s="16">
+        <v>5</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="15">
-        <v>57</v>
-      </c>
-      <c r="C16" s="15">
-        <v>5</v>
-      </c>
-      <c r="D16" s="16">
+      <c r="A16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="14">
+        <v>57</v>
+      </c>
+      <c r="C16" s="14">
+        <v>5</v>
+      </c>
+      <c r="D16" s="15">
         <v>15</v>
       </c>
-      <c r="E16" s="17">
-        <v>5</v>
-      </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="E16" s="16">
+        <v>5</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="15">
-        <v>57</v>
-      </c>
-      <c r="C17" s="15">
-        <v>5</v>
-      </c>
-      <c r="D17" s="16">
+      <c r="A17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="14">
+        <v>57</v>
+      </c>
+      <c r="C17" s="14">
+        <v>5</v>
+      </c>
+      <c r="D17" s="15">
         <v>16</v>
       </c>
-      <c r="E17" s="17">
-        <v>4</v>
-      </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
+      <c r="E17" s="16">
+        <v>4</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="15">
-        <v>57</v>
-      </c>
-      <c r="C18" s="15">
-        <v>5</v>
-      </c>
-      <c r="D18" s="16">
+      <c r="A18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="14">
+        <v>57</v>
+      </c>
+      <c r="C18" s="14">
+        <v>5</v>
+      </c>
+      <c r="D18" s="15">
         <v>17</v>
       </c>
-      <c r="E18" s="17">
-        <v>4</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="E18" s="16">
+        <v>4</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="15">
-        <v>57</v>
-      </c>
-      <c r="C19" s="15">
-        <v>5</v>
-      </c>
-      <c r="D19" s="16">
+      <c r="A19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="14">
+        <v>57</v>
+      </c>
+      <c r="C19" s="14">
+        <v>5</v>
+      </c>
+      <c r="D19" s="15">
         <v>18</v>
       </c>
-      <c r="E19" s="17">
-        <v>4</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
+      <c r="E19" s="16">
+        <v>4</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="15">
-        <v>57</v>
-      </c>
-      <c r="C20" s="15">
-        <v>5</v>
-      </c>
-      <c r="D20" s="16">
+      <c r="A20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="14">
+        <v>57</v>
+      </c>
+      <c r="C20" s="14">
+        <v>5</v>
+      </c>
+      <c r="D20" s="15">
         <v>19</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="16">
         <v>3</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2469,8 +2905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2616C2C6-9D9A-D343-91E5-FA4920B1432D}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C2:C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2479,407 +2915,1690 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="13" t="s">
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="15">
-        <v>57</v>
-      </c>
-      <c r="C2" s="15">
-        <v>6</v>
-      </c>
-      <c r="D2" s="16">
+      <c r="A2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14">
+        <v>57</v>
+      </c>
+      <c r="C2" s="14">
+        <v>6</v>
+      </c>
+      <c r="D2" s="15">
         <v>1</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <v>2</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="15">
-        <v>57</v>
-      </c>
-      <c r="C3" s="15">
-        <v>6</v>
-      </c>
-      <c r="D3" s="16">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="14">
+        <v>57</v>
+      </c>
+      <c r="C3" s="14">
+        <v>6</v>
+      </c>
+      <c r="D3" s="15">
         <v>2</v>
       </c>
-      <c r="E3" s="17">
-        <v>4</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="E3" s="16">
+        <v>4</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="15">
-        <v>57</v>
-      </c>
-      <c r="C4" s="15">
-        <v>6</v>
-      </c>
-      <c r="D4" s="16">
+      <c r="A4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="14">
+        <v>57</v>
+      </c>
+      <c r="C4" s="14">
+        <v>6</v>
+      </c>
+      <c r="D4" s="15">
         <v>3</v>
       </c>
-      <c r="E4" s="17">
-        <v>5</v>
-      </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="16">
+        <v>5</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="15">
-        <v>57</v>
-      </c>
-      <c r="C5" s="15">
-        <v>6</v>
-      </c>
-      <c r="D5" s="16">
-        <v>4</v>
-      </c>
-      <c r="E5" s="17">
-        <v>5</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="A5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="14">
+        <v>57</v>
+      </c>
+      <c r="C5" s="14">
+        <v>6</v>
+      </c>
+      <c r="D5" s="15">
+        <v>4</v>
+      </c>
+      <c r="E5" s="16">
+        <v>5</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="15">
-        <v>57</v>
-      </c>
-      <c r="C6" s="15">
-        <v>6</v>
-      </c>
-      <c r="D6" s="16">
-        <v>5</v>
-      </c>
-      <c r="E6" s="17">
-        <v>5</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14">
+        <v>57</v>
+      </c>
+      <c r="C6" s="14">
+        <v>6</v>
+      </c>
+      <c r="D6" s="15">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <v>5</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="15">
-        <v>57</v>
-      </c>
-      <c r="C7" s="15">
-        <v>6</v>
-      </c>
-      <c r="D7" s="16">
-        <v>6</v>
-      </c>
-      <c r="E7" s="17">
-        <v>5</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="A7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="14">
+        <v>57</v>
+      </c>
+      <c r="C7" s="14">
+        <v>6</v>
+      </c>
+      <c r="D7" s="15">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16">
+        <v>5</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="15">
-        <v>57</v>
-      </c>
-      <c r="C8" s="15">
-        <v>6</v>
-      </c>
-      <c r="D8" s="16">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14">
+        <v>57</v>
+      </c>
+      <c r="C8" s="14">
+        <v>6</v>
+      </c>
+      <c r="D8" s="15">
         <v>7</v>
       </c>
-      <c r="E8" s="17">
-        <v>5</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="E8" s="16">
+        <v>5</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="15">
-        <v>57</v>
-      </c>
-      <c r="C9" s="15">
-        <v>6</v>
-      </c>
-      <c r="D9" s="16">
+      <c r="A9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14">
+        <v>57</v>
+      </c>
+      <c r="C9" s="14">
+        <v>6</v>
+      </c>
+      <c r="D9" s="15">
         <v>8</v>
       </c>
-      <c r="E9" s="17">
-        <v>6</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="E9" s="16">
+        <v>6</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="15">
-        <v>57</v>
-      </c>
-      <c r="C10" s="15">
-        <v>6</v>
-      </c>
-      <c r="D10" s="16">
-        <v>9</v>
-      </c>
-      <c r="E10" s="17">
-        <v>6</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="A10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>57</v>
+      </c>
+      <c r="C10" s="14">
+        <v>6</v>
+      </c>
+      <c r="D10" s="15">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16">
+        <v>6</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="15">
-        <v>57</v>
-      </c>
-      <c r="C11" s="15">
-        <v>6</v>
-      </c>
-      <c r="D11" s="16">
-        <v>10</v>
-      </c>
-      <c r="E11" s="17">
-        <v>6</v>
-      </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+      <c r="A11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14">
+        <v>6</v>
+      </c>
+      <c r="D11" s="15">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16">
+        <v>6</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="15">
-        <v>57</v>
-      </c>
-      <c r="C12" s="15">
-        <v>6</v>
-      </c>
-      <c r="D12" s="16">
+      <c r="A12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14">
+        <v>57</v>
+      </c>
+      <c r="C12" s="14">
+        <v>6</v>
+      </c>
+      <c r="D12" s="15">
         <v>11</v>
       </c>
-      <c r="E12" s="17">
-        <v>6</v>
-      </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="E12" s="16">
+        <v>6</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="15">
-        <v>57</v>
-      </c>
-      <c r="C13" s="15">
-        <v>6</v>
-      </c>
-      <c r="D13" s="16">
+      <c r="A13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14">
+        <v>57</v>
+      </c>
+      <c r="C13" s="14">
+        <v>6</v>
+      </c>
+      <c r="D13" s="15">
         <v>12</v>
       </c>
-      <c r="E13" s="17">
-        <v>5</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="E13" s="16">
+        <v>5</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="15">
-        <v>57</v>
-      </c>
-      <c r="C14" s="15">
-        <v>6</v>
-      </c>
-      <c r="D14" s="16">
+      <c r="A14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="14">
+        <v>57</v>
+      </c>
+      <c r="C14" s="14">
+        <v>6</v>
+      </c>
+      <c r="D14" s="15">
         <v>13</v>
       </c>
-      <c r="E14" s="17">
-        <v>5</v>
-      </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="E14" s="16">
+        <v>5</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="15">
-        <v>57</v>
-      </c>
-      <c r="C15" s="15">
-        <v>6</v>
-      </c>
-      <c r="D15" s="16">
+      <c r="A15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="14">
+        <v>57</v>
+      </c>
+      <c r="C15" s="14">
+        <v>6</v>
+      </c>
+      <c r="D15" s="15">
         <v>14</v>
       </c>
-      <c r="E15" s="17">
-        <v>5</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="E15" s="16">
+        <v>5</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="15">
-        <v>57</v>
-      </c>
-      <c r="C16" s="15">
-        <v>6</v>
-      </c>
-      <c r="D16" s="16">
+      <c r="A16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="14">
+        <v>57</v>
+      </c>
+      <c r="C16" s="14">
+        <v>6</v>
+      </c>
+      <c r="D16" s="15">
         <v>15</v>
       </c>
-      <c r="E16" s="17">
-        <v>5</v>
-      </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="E16" s="16">
+        <v>5</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="15">
-        <v>57</v>
-      </c>
-      <c r="C17" s="15">
-        <v>6</v>
-      </c>
-      <c r="D17" s="16">
+      <c r="A17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="14">
+        <v>57</v>
+      </c>
+      <c r="C17" s="14">
+        <v>6</v>
+      </c>
+      <c r="D17" s="15">
         <v>16</v>
       </c>
-      <c r="E17" s="17">
-        <v>5</v>
-      </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
+      <c r="E17" s="16">
+        <v>5</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="15">
-        <v>57</v>
-      </c>
-      <c r="C18" s="15">
-        <v>6</v>
-      </c>
-      <c r="D18" s="16">
+      <c r="A18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="14">
+        <v>57</v>
+      </c>
+      <c r="C18" s="14">
+        <v>6</v>
+      </c>
+      <c r="D18" s="15">
         <v>17</v>
       </c>
-      <c r="E18" s="17">
-        <v>5</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="E18" s="16">
+        <v>5</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="15">
-        <v>57</v>
-      </c>
-      <c r="C19" s="15">
-        <v>6</v>
-      </c>
-      <c r="D19" s="16">
+      <c r="A19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="14">
+        <v>57</v>
+      </c>
+      <c r="C19" s="14">
+        <v>6</v>
+      </c>
+      <c r="D19" s="15">
         <v>18</v>
       </c>
-      <c r="E19" s="17">
-        <v>4</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
+      <c r="E19" s="16">
+        <v>4</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="15">
-        <v>57</v>
-      </c>
-      <c r="C20" s="15">
-        <v>6</v>
-      </c>
-      <c r="D20" s="16">
+      <c r="A20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="14">
+        <v>57</v>
+      </c>
+      <c r="C20" s="14">
+        <v>6</v>
+      </c>
+      <c r="D20" s="15">
         <v>19</v>
       </c>
-      <c r="E20" s="17">
-        <v>4</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="E20" s="16">
+        <v>4</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BF220A-C859-1142-B4BD-F1040CB025E7}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14">
+        <v>57</v>
+      </c>
+      <c r="C2" s="14">
+        <v>7</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="14">
+        <v>57</v>
+      </c>
+      <c r="C3" s="14">
+        <v>7</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2</v>
+      </c>
+      <c r="E3" s="16">
+        <v>3</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="14">
+        <v>57</v>
+      </c>
+      <c r="C4" s="14">
+        <v>7</v>
+      </c>
+      <c r="D4" s="15">
+        <v>3</v>
+      </c>
+      <c r="E4" s="16">
+        <v>4</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="14">
+        <v>57</v>
+      </c>
+      <c r="C5" s="14">
+        <v>7</v>
+      </c>
+      <c r="D5" s="15">
+        <v>4</v>
+      </c>
+      <c r="E5" s="16">
+        <v>4</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14">
+        <v>57</v>
+      </c>
+      <c r="C6" s="14">
+        <v>7</v>
+      </c>
+      <c r="D6" s="15">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <v>4</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="14">
+        <v>57</v>
+      </c>
+      <c r="C7" s="14">
+        <v>7</v>
+      </c>
+      <c r="D7" s="15">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16">
+        <v>5</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14">
+        <v>57</v>
+      </c>
+      <c r="C8" s="14">
+        <v>7</v>
+      </c>
+      <c r="D8" s="15">
+        <v>7</v>
+      </c>
+      <c r="E8" s="16">
+        <v>6</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14">
+        <v>57</v>
+      </c>
+      <c r="C9" s="14">
+        <v>7</v>
+      </c>
+      <c r="D9" s="15">
+        <v>8</v>
+      </c>
+      <c r="E9" s="16">
+        <v>6</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>57</v>
+      </c>
+      <c r="C10" s="14">
+        <v>7</v>
+      </c>
+      <c r="D10" s="15">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16">
+        <v>6</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14">
+        <v>7</v>
+      </c>
+      <c r="D11" s="15">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16">
+        <v>6</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14">
+        <v>57</v>
+      </c>
+      <c r="C12" s="14">
+        <v>7</v>
+      </c>
+      <c r="D12" s="15">
+        <v>11</v>
+      </c>
+      <c r="E12" s="16">
+        <v>6</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14">
+        <v>57</v>
+      </c>
+      <c r="C13" s="14">
+        <v>7</v>
+      </c>
+      <c r="D13" s="15">
+        <v>12</v>
+      </c>
+      <c r="E13" s="16">
+        <v>6</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="14">
+        <v>57</v>
+      </c>
+      <c r="C14" s="14">
+        <v>7</v>
+      </c>
+      <c r="D14" s="15">
+        <v>13</v>
+      </c>
+      <c r="E14" s="16">
+        <v>5</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="14">
+        <v>57</v>
+      </c>
+      <c r="C15" s="14">
+        <v>7</v>
+      </c>
+      <c r="D15" s="15">
+        <v>14</v>
+      </c>
+      <c r="E15" s="16">
+        <v>5</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="14">
+        <v>57</v>
+      </c>
+      <c r="C16" s="14">
+        <v>7</v>
+      </c>
+      <c r="D16" s="15">
+        <v>15</v>
+      </c>
+      <c r="E16" s="16">
+        <v>5</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="14">
+        <v>57</v>
+      </c>
+      <c r="C17" s="14">
+        <v>7</v>
+      </c>
+      <c r="D17" s="15">
+        <v>16</v>
+      </c>
+      <c r="E17" s="16">
+        <v>5</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="14">
+        <v>57</v>
+      </c>
+      <c r="C18" s="14">
+        <v>7</v>
+      </c>
+      <c r="D18" s="15">
+        <v>17</v>
+      </c>
+      <c r="E18" s="16">
+        <v>5</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="14">
+        <v>57</v>
+      </c>
+      <c r="C19" s="14">
+        <v>7</v>
+      </c>
+      <c r="D19" s="15">
+        <v>18</v>
+      </c>
+      <c r="E19" s="16">
+        <v>4</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="14">
+        <v>57</v>
+      </c>
+      <c r="C20" s="14">
+        <v>7</v>
+      </c>
+      <c r="D20" s="15">
+        <v>19</v>
+      </c>
+      <c r="E20" s="16">
+        <v>4</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8C9AE9-A34E-0340-9A18-D5374AF02AB3}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14">
+        <v>57</v>
+      </c>
+      <c r="C2" s="14">
+        <v>8</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="14">
+        <v>57</v>
+      </c>
+      <c r="C3" s="14">
+        <v>8</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2</v>
+      </c>
+      <c r="E3" s="16">
+        <v>3</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="14">
+        <v>57</v>
+      </c>
+      <c r="C4" s="14">
+        <v>8</v>
+      </c>
+      <c r="D4" s="15">
+        <v>3</v>
+      </c>
+      <c r="E4" s="16">
+        <v>5</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="14">
+        <v>57</v>
+      </c>
+      <c r="C5" s="14">
+        <v>8</v>
+      </c>
+      <c r="D5" s="15">
+        <v>4</v>
+      </c>
+      <c r="E5" s="16">
+        <v>5</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14">
+        <v>57</v>
+      </c>
+      <c r="C6" s="14">
+        <v>8</v>
+      </c>
+      <c r="D6" s="15">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <v>5</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="14">
+        <v>57</v>
+      </c>
+      <c r="C7" s="14">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16">
+        <v>6</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14">
+        <v>57</v>
+      </c>
+      <c r="C8" s="14">
+        <v>8</v>
+      </c>
+      <c r="D8" s="15">
+        <v>7</v>
+      </c>
+      <c r="E8" s="16">
+        <v>6</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14">
+        <v>57</v>
+      </c>
+      <c r="C9" s="14">
+        <v>8</v>
+      </c>
+      <c r="D9" s="15">
+        <v>8</v>
+      </c>
+      <c r="E9" s="16">
+        <v>6</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>57</v>
+      </c>
+      <c r="C10" s="14">
+        <v>8</v>
+      </c>
+      <c r="D10" s="15">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16">
+        <v>6</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14">
+        <v>8</v>
+      </c>
+      <c r="D11" s="15">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16">
+        <v>6</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14">
+        <v>57</v>
+      </c>
+      <c r="C12" s="14">
+        <v>8</v>
+      </c>
+      <c r="D12" s="15">
+        <v>11</v>
+      </c>
+      <c r="E12" s="16">
+        <v>6</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14">
+        <v>57</v>
+      </c>
+      <c r="C13" s="14">
+        <v>8</v>
+      </c>
+      <c r="D13" s="15">
+        <v>12</v>
+      </c>
+      <c r="E13" s="16">
+        <v>6</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="14">
+        <v>57</v>
+      </c>
+      <c r="C14" s="14">
+        <v>8</v>
+      </c>
+      <c r="D14" s="15">
+        <v>13</v>
+      </c>
+      <c r="E14" s="16">
+        <v>5</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="14">
+        <v>57</v>
+      </c>
+      <c r="C15" s="14">
+        <v>8</v>
+      </c>
+      <c r="D15" s="15">
+        <v>14</v>
+      </c>
+      <c r="E15" s="16">
+        <v>5</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="14">
+        <v>57</v>
+      </c>
+      <c r="C16" s="14">
+        <v>8</v>
+      </c>
+      <c r="D16" s="15">
+        <v>15</v>
+      </c>
+      <c r="E16" s="16">
+        <v>5</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="14">
+        <v>57</v>
+      </c>
+      <c r="C17" s="14">
+        <v>8</v>
+      </c>
+      <c r="D17" s="15">
+        <v>16</v>
+      </c>
+      <c r="E17" s="16">
+        <v>5</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="14">
+        <v>57</v>
+      </c>
+      <c r="C18" s="14">
+        <v>8</v>
+      </c>
+      <c r="D18" s="15">
+        <v>17</v>
+      </c>
+      <c r="E18" s="16">
+        <v>4</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="14">
+        <v>57</v>
+      </c>
+      <c r="C19" s="14">
+        <v>8</v>
+      </c>
+      <c r="D19" s="15">
+        <v>18</v>
+      </c>
+      <c r="E19" s="16">
+        <v>4</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="14">
+        <v>57</v>
+      </c>
+      <c r="C20" s="14">
+        <v>8</v>
+      </c>
+      <c r="D20" s="15">
+        <v>19</v>
+      </c>
+      <c r="E20" s="16">
+        <v>4</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D716B64-018C-6746-A03A-DCA360F54B17}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14">
+        <v>57</v>
+      </c>
+      <c r="C2" s="14">
+        <v>9</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="14">
+        <v>57</v>
+      </c>
+      <c r="C3" s="14">
+        <v>9</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2</v>
+      </c>
+      <c r="E3" s="16">
+        <v>3</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="14">
+        <v>57</v>
+      </c>
+      <c r="C4" s="14">
+        <v>9</v>
+      </c>
+      <c r="D4" s="15">
+        <v>3</v>
+      </c>
+      <c r="E4" s="16">
+        <v>4</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="14">
+        <v>57</v>
+      </c>
+      <c r="C5" s="14">
+        <v>9</v>
+      </c>
+      <c r="D5" s="15">
+        <v>4</v>
+      </c>
+      <c r="E5" s="16">
+        <v>5</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14">
+        <v>57</v>
+      </c>
+      <c r="C6" s="14">
+        <v>9</v>
+      </c>
+      <c r="D6" s="15">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <v>5</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="14">
+        <v>57</v>
+      </c>
+      <c r="C7" s="14">
+        <v>9</v>
+      </c>
+      <c r="D7" s="15">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16">
+        <v>5</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14">
+        <v>57</v>
+      </c>
+      <c r="C8" s="14">
+        <v>9</v>
+      </c>
+      <c r="D8" s="15">
+        <v>7</v>
+      </c>
+      <c r="E8" s="16">
+        <v>5</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14">
+        <v>57</v>
+      </c>
+      <c r="C9" s="14">
+        <v>9</v>
+      </c>
+      <c r="D9" s="15">
+        <v>8</v>
+      </c>
+      <c r="E9" s="16">
+        <v>6</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>57</v>
+      </c>
+      <c r="C10" s="14">
+        <v>9</v>
+      </c>
+      <c r="D10" s="15">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16">
+        <v>6</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14">
+        <v>9</v>
+      </c>
+      <c r="D11" s="15">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16">
+        <v>6</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14">
+        <v>57</v>
+      </c>
+      <c r="C12" s="14">
+        <v>9</v>
+      </c>
+      <c r="D12" s="15">
+        <v>11</v>
+      </c>
+      <c r="E12" s="16">
+        <v>6</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14">
+        <v>57</v>
+      </c>
+      <c r="C13" s="14">
+        <v>9</v>
+      </c>
+      <c r="D13" s="15">
+        <v>12</v>
+      </c>
+      <c r="E13" s="16">
+        <v>5</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="14">
+        <v>57</v>
+      </c>
+      <c r="C14" s="14">
+        <v>9</v>
+      </c>
+      <c r="D14" s="15">
+        <v>13</v>
+      </c>
+      <c r="E14" s="16">
+        <v>5</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="14">
+        <v>57</v>
+      </c>
+      <c r="C15" s="14">
+        <v>9</v>
+      </c>
+      <c r="D15" s="15">
+        <v>14</v>
+      </c>
+      <c r="E15" s="16">
+        <v>5</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="14">
+        <v>57</v>
+      </c>
+      <c r="C16" s="14">
+        <v>9</v>
+      </c>
+      <c r="D16" s="15">
+        <v>15</v>
+      </c>
+      <c r="E16" s="16">
+        <v>5</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="14">
+        <v>57</v>
+      </c>
+      <c r="C17" s="14">
+        <v>9</v>
+      </c>
+      <c r="D17" s="15">
+        <v>16</v>
+      </c>
+      <c r="E17" s="16">
+        <v>5</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="14">
+        <v>57</v>
+      </c>
+      <c r="C18" s="14">
+        <v>9</v>
+      </c>
+      <c r="D18" s="15">
+        <v>17</v>
+      </c>
+      <c r="E18" s="16">
+        <v>4</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="14">
+        <v>57</v>
+      </c>
+      <c r="C19" s="14">
+        <v>9</v>
+      </c>
+      <c r="D19" s="15">
+        <v>18</v>
+      </c>
+      <c r="E19" s="16">
+        <v>4</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="14">
+        <v>57</v>
+      </c>
+      <c r="C20" s="14">
+        <v>9</v>
+      </c>
+      <c r="D20" s="15">
+        <v>19</v>
+      </c>
+      <c r="E20" s="16">
+        <v>4</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="14">
+        <v>57</v>
+      </c>
+      <c r="C21" s="14">
+        <v>9</v>
+      </c>
+      <c r="D21" s="15">
+        <v>20</v>
+      </c>
+      <c r="E21" s="19">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>